<commit_message>
32-ims-changes and table created
</commit_message>
<xml_diff>
--- a/info-ims.xlsx
+++ b/info-ims.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="149">
   <si>
     <t>DESCRIBE application</t>
   </si>
@@ -406,6 +406,63 @@
   </si>
   <si>
     <t>changed_at</t>
+  </si>
+  <si>
+    <t>DESCRIBE enrollments</t>
+  </si>
+  <si>
+    <t>referralid</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>enrollmentdate</t>
+  </si>
+  <si>
+    <t>fee_paid</t>
+  </si>
+  <si>
+    <t>DESCRIBE payments</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>payment_date</t>
+  </si>
+  <si>
+    <t>enum('Pending','Completed','Failed')</t>
+  </si>
+  <si>
+    <t>DESCRIBE referrals</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>referred_email</t>
+  </si>
+  <si>
+    <t>referred_phone</t>
+  </si>
+  <si>
+    <t>enum('Pending','Enrolled','Paid')</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>DESCRIBE students</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>referral_code</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
   </si>
 </sst>
 </file>
@@ -421,7 +478,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +527,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -483,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -492,6 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S177"/>
+  <dimension ref="A1:Y213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="J164" sqref="J164"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="I205" sqref="I205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4664,7 +4728,7 @@
       <c r="R158" s="4"/>
       <c r="S158" s="4"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4674,8 +4738,16 @@
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L162" s="1"/>
+      <c r="M162" s="1"/>
+      <c r="N162" s="1"/>
+      <c r="O162" s="1"/>
+      <c r="P162" s="1"/>
+      <c r="Q162" s="1"/>
+      <c r="R162" s="1"/>
+      <c r="S162" s="1"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4685,8 +4757,16 @@
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L163" s="1"/>
+      <c r="M163" s="1"/>
+      <c r="N163" s="1"/>
+      <c r="O163" s="1"/>
+      <c r="P163" s="1"/>
+      <c r="Q163" s="1"/>
+      <c r="R163" s="1"/>
+      <c r="S163" s="1"/>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4696,8 +4776,16 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L164" s="1"/>
+      <c r="M164" s="1"/>
+      <c r="N164" s="1"/>
+      <c r="O164" s="1"/>
+      <c r="P164" s="1"/>
+      <c r="Q164" s="1"/>
+      <c r="R164" s="1"/>
+      <c r="S164" s="1"/>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>124</v>
       </c>
@@ -4709,8 +4797,16 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L165" s="1"/>
+      <c r="M165" s="1"/>
+      <c r="N165" s="1"/>
+      <c r="O165" s="1"/>
+      <c r="P165" s="1"/>
+      <c r="Q165" s="1"/>
+      <c r="R165" s="1"/>
+      <c r="S165" s="1"/>
+    </row>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4720,8 +4816,16 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L166" s="1"/>
+      <c r="M166" s="1"/>
+      <c r="N166" s="1"/>
+      <c r="O166" s="1"/>
+      <c r="P166" s="1"/>
+      <c r="Q166" s="1"/>
+      <c r="R166" s="1"/>
+      <c r="S166" s="1"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4731,8 +4835,18 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L167" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M167" s="1"/>
+      <c r="N167" s="1"/>
+      <c r="O167" s="1"/>
+      <c r="P167" s="1"/>
+      <c r="Q167" s="1"/>
+      <c r="R167" s="1"/>
+      <c r="S167" s="1"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4742,8 +4856,16 @@
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L168" s="1"/>
+      <c r="M168" s="1"/>
+      <c r="N168" s="1"/>
+      <c r="O168" s="1"/>
+      <c r="P168" s="1"/>
+      <c r="Q168" s="1"/>
+      <c r="R168" s="1"/>
+      <c r="S168" s="1"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>1</v>
       </c>
@@ -4765,8 +4887,16 @@
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L169" s="1"/>
+      <c r="M169" s="1"/>
+      <c r="N169" s="1"/>
+      <c r="O169" s="1"/>
+      <c r="P169" s="1"/>
+      <c r="Q169" s="1"/>
+      <c r="R169" s="1"/>
+      <c r="S169" s="1"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>123</v>
       </c>
@@ -4786,8 +4916,16 @@
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L170" s="1"/>
+      <c r="M170" s="1"/>
+      <c r="N170" s="1"/>
+      <c r="O170" s="1"/>
+      <c r="P170" s="1"/>
+      <c r="Q170" s="1"/>
+      <c r="R170" s="1"/>
+      <c r="S170" s="1"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>125</v>
       </c>
@@ -4807,8 +4945,28 @@
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L171" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M171" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N171" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O171" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P171" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R171" s="1"/>
+      <c r="S171" s="1"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>126</v>
       </c>
@@ -4826,8 +4984,26 @@
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L172" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M172" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N172" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O172" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P172" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q172" s="1"/>
+      <c r="R172" s="1"/>
+      <c r="S172" s="1"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>127</v>
       </c>
@@ -4845,8 +5021,24 @@
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L173" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M173" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N173" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O173" s="1"/>
+      <c r="P173" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q173" s="1"/>
+      <c r="R173" s="1"/>
+      <c r="S173" s="1"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>128</v>
       </c>
@@ -4864,8 +5056,24 @@
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L174" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N174" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O174" s="1"/>
+      <c r="P174" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q174" s="1"/>
+      <c r="R174" s="1"/>
+      <c r="S174" s="1"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>129</v>
       </c>
@@ -4883,8 +5091,24 @@
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L175" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M175" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N175" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O175" s="1"/>
+      <c r="P175" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q175" s="1"/>
+      <c r="R175" s="1"/>
+      <c r="S175" s="1"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4894,8 +5118,16 @@
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L176" s="1"/>
+      <c r="M176" s="1"/>
+      <c r="N176" s="1"/>
+      <c r="O176" s="1"/>
+      <c r="P176" s="1"/>
+      <c r="Q176" s="1"/>
+      <c r="R176" s="1"/>
+      <c r="S176" s="1"/>
+    </row>
+    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4905,6 +5137,726 @@
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
+      <c r="L177" s="1"/>
+      <c r="M177" s="1"/>
+      <c r="N177" s="1"/>
+      <c r="O177" s="1"/>
+      <c r="P177" s="1"/>
+      <c r="Q177" s="1"/>
+      <c r="R177" s="1"/>
+      <c r="S177" s="1"/>
+    </row>
+    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A180" s="2"/>
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2"/>
+      <c r="F180" s="2"/>
+      <c r="G180" s="2"/>
+      <c r="H180" s="2"/>
+      <c r="I180" s="2"/>
+      <c r="J180" s="2"/>
+      <c r="K180" s="2"/>
+      <c r="L180" s="2"/>
+      <c r="N180" s="8"/>
+      <c r="O180" s="8"/>
+      <c r="P180" s="8"/>
+      <c r="Q180" s="8"/>
+      <c r="R180" s="8"/>
+      <c r="S180" s="8"/>
+      <c r="T180" s="8"/>
+      <c r="U180" s="8"/>
+      <c r="V180" s="8"/>
+      <c r="W180" s="8"/>
+      <c r="X180" s="8"/>
+      <c r="Y180" s="8"/>
+    </row>
+    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A181" s="2"/>
+      <c r="B181" s="2"/>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
+      <c r="F181" s="2"/>
+      <c r="G181" s="2"/>
+      <c r="H181" s="2"/>
+      <c r="I181" s="2"/>
+      <c r="J181" s="2"/>
+      <c r="K181" s="2"/>
+      <c r="L181" s="2"/>
+      <c r="N181" s="8"/>
+      <c r="O181" s="8"/>
+      <c r="P181" s="8"/>
+      <c r="Q181" s="8"/>
+      <c r="R181" s="8"/>
+      <c r="S181" s="8"/>
+      <c r="T181" s="8"/>
+      <c r="U181" s="8"/>
+      <c r="V181" s="8"/>
+      <c r="W181" s="8"/>
+      <c r="X181" s="8"/>
+      <c r="Y181" s="8"/>
+    </row>
+    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A182" s="2"/>
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="2"/>
+      <c r="F182" s="2"/>
+      <c r="G182" s="2"/>
+      <c r="H182" s="2"/>
+      <c r="I182" s="2"/>
+      <c r="J182" s="2"/>
+      <c r="K182" s="2"/>
+      <c r="L182" s="2"/>
+      <c r="N182" s="8"/>
+      <c r="O182" s="8"/>
+      <c r="P182" s="8"/>
+      <c r="Q182" s="8"/>
+      <c r="R182" s="8"/>
+      <c r="S182" s="8"/>
+      <c r="T182" s="8"/>
+      <c r="U182" s="8"/>
+      <c r="V182" s="8"/>
+      <c r="W182" s="8"/>
+      <c r="X182" s="8"/>
+      <c r="Y182" s="8"/>
+    </row>
+    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A183" s="2"/>
+      <c r="B183" s="2"/>
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
+      <c r="E183" s="2"/>
+      <c r="F183" s="2"/>
+      <c r="G183" s="2"/>
+      <c r="H183" s="2"/>
+      <c r="I183" s="2"/>
+      <c r="J183" s="2"/>
+      <c r="K183" s="2"/>
+      <c r="L183" s="2"/>
+      <c r="N183" s="8"/>
+      <c r="O183" s="8"/>
+      <c r="P183" s="8"/>
+      <c r="Q183" s="8"/>
+      <c r="R183" s="8"/>
+      <c r="S183" s="8"/>
+      <c r="T183" s="8"/>
+      <c r="U183" s="8"/>
+      <c r="V183" s="8"/>
+      <c r="W183" s="8"/>
+      <c r="X183" s="8"/>
+      <c r="Y183" s="8"/>
+    </row>
+    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A184" s="2"/>
+      <c r="B184" s="2"/>
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
+      <c r="E184" s="2"/>
+      <c r="F184" s="2"/>
+      <c r="G184" s="2"/>
+      <c r="H184" s="2"/>
+      <c r="I184" s="2"/>
+      <c r="J184" s="2"/>
+      <c r="K184" s="2"/>
+      <c r="L184" s="2"/>
+      <c r="N184" s="8"/>
+      <c r="O184" s="8"/>
+      <c r="P184" s="8"/>
+      <c r="Q184" s="8"/>
+      <c r="R184" s="8"/>
+      <c r="S184" s="8"/>
+      <c r="T184" s="8"/>
+      <c r="U184" s="8"/>
+      <c r="V184" s="8"/>
+      <c r="W184" s="8"/>
+      <c r="X184" s="8"/>
+      <c r="Y184" s="8"/>
+    </row>
+    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
+      <c r="D185" s="2"/>
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
+      <c r="G185" s="2"/>
+      <c r="H185" s="2"/>
+      <c r="I185" s="2"/>
+      <c r="J185" s="2"/>
+      <c r="K185" s="2"/>
+      <c r="L185" s="2"/>
+      <c r="N185" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="O185" s="8"/>
+      <c r="P185" s="8"/>
+      <c r="Q185" s="8"/>
+      <c r="R185" s="8"/>
+      <c r="S185" s="8"/>
+      <c r="T185" s="8"/>
+      <c r="U185" s="8"/>
+      <c r="V185" s="8"/>
+      <c r="W185" s="8"/>
+      <c r="X185" s="8"/>
+      <c r="Y185" s="8"/>
+    </row>
+    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A186" s="2"/>
+      <c r="B186" s="2"/>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
+      <c r="E186" s="2"/>
+      <c r="F186" s="2"/>
+      <c r="G186" s="2"/>
+      <c r="H186" s="2"/>
+      <c r="I186" s="2"/>
+      <c r="J186" s="2"/>
+      <c r="K186" s="2"/>
+      <c r="L186" s="2"/>
+      <c r="N186" s="8"/>
+      <c r="O186" s="8"/>
+      <c r="P186" s="8"/>
+      <c r="Q186" s="8"/>
+      <c r="R186" s="8"/>
+      <c r="S186" s="8"/>
+      <c r="T186" s="8"/>
+      <c r="U186" s="8"/>
+      <c r="V186" s="8"/>
+      <c r="W186" s="8"/>
+      <c r="X186" s="8"/>
+      <c r="Y186" s="8"/>
+    </row>
+    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A187" s="2"/>
+      <c r="B187" s="2"/>
+      <c r="C187" s="2"/>
+      <c r="D187" s="2"/>
+      <c r="E187" s="2"/>
+      <c r="F187" s="2"/>
+      <c r="G187" s="2"/>
+      <c r="H187" s="2"/>
+      <c r="I187" s="2"/>
+      <c r="J187" s="2"/>
+      <c r="K187" s="2"/>
+      <c r="L187" s="2"/>
+      <c r="N187" s="8"/>
+      <c r="O187" s="8"/>
+      <c r="P187" s="8"/>
+      <c r="Q187" s="8"/>
+      <c r="R187" s="8"/>
+      <c r="S187" s="8"/>
+      <c r="T187" s="8"/>
+      <c r="U187" s="8"/>
+      <c r="V187" s="8"/>
+      <c r="W187" s="8"/>
+      <c r="X187" s="8"/>
+      <c r="Y187" s="8"/>
+    </row>
+    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A188" s="2"/>
+      <c r="B188" s="2"/>
+      <c r="C188" s="2"/>
+      <c r="D188" s="2"/>
+      <c r="E188" s="2"/>
+      <c r="F188" s="2"/>
+      <c r="G188" s="2"/>
+      <c r="H188" s="2"/>
+      <c r="I188" s="2"/>
+      <c r="J188" s="2"/>
+      <c r="K188" s="2"/>
+      <c r="L188" s="2"/>
+      <c r="N188" s="8"/>
+      <c r="O188" s="8"/>
+      <c r="P188" s="8"/>
+      <c r="Q188" s="8"/>
+      <c r="R188" s="8"/>
+      <c r="S188" s="8"/>
+      <c r="T188" s="8"/>
+      <c r="U188" s="8"/>
+      <c r="V188" s="8"/>
+      <c r="W188" s="8"/>
+      <c r="X188" s="8"/>
+      <c r="Y188" s="8"/>
+    </row>
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G189" s="2"/>
+      <c r="H189" s="2"/>
+      <c r="I189" s="2"/>
+      <c r="J189" s="2"/>
+      <c r="K189" s="2"/>
+      <c r="L189" s="2"/>
+      <c r="N189" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O189" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P189" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q189" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R189" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S189" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T189" s="8"/>
+      <c r="U189" s="8"/>
+      <c r="V189" s="8"/>
+      <c r="W189" s="8"/>
+      <c r="X189" s="8"/>
+      <c r="Y189" s="8"/>
+    </row>
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F190" s="2"/>
+      <c r="G190" s="2"/>
+      <c r="H190" s="2"/>
+      <c r="I190" s="2"/>
+      <c r="J190" s="2"/>
+      <c r="K190" s="2"/>
+      <c r="L190" s="2"/>
+      <c r="N190" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="O190" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P190" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q190" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="R190" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S190" s="8"/>
+      <c r="T190" s="8"/>
+      <c r="U190" s="8"/>
+      <c r="V190" s="8"/>
+      <c r="W190" s="8"/>
+      <c r="X190" s="8"/>
+      <c r="Y190" s="8"/>
+    </row>
+    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D191" s="2"/>
+      <c r="E191" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F191" s="2"/>
+      <c r="G191" s="2"/>
+      <c r="H191" s="2"/>
+      <c r="I191" s="2"/>
+      <c r="J191" s="2"/>
+      <c r="K191" s="2"/>
+      <c r="L191" s="2"/>
+      <c r="N191" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="O191" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P191" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q191" s="8"/>
+      <c r="R191" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S191" s="8"/>
+      <c r="T191" s="8"/>
+      <c r="U191" s="8"/>
+      <c r="V191" s="8"/>
+      <c r="W191" s="8"/>
+      <c r="X191" s="8"/>
+      <c r="Y191" s="8"/>
+    </row>
+    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D192" s="2"/>
+      <c r="E192" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F192" s="2"/>
+      <c r="G192" s="2"/>
+      <c r="H192" s="2"/>
+      <c r="I192" s="2"/>
+      <c r="J192" s="2"/>
+      <c r="K192" s="2"/>
+      <c r="L192" s="2"/>
+      <c r="N192" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="O192" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P192" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q192" s="8"/>
+      <c r="R192" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S192" s="8"/>
+      <c r="T192" s="8"/>
+      <c r="U192" s="8"/>
+      <c r="V192" s="8"/>
+      <c r="W192" s="8"/>
+      <c r="X192" s="8"/>
+      <c r="Y192" s="8"/>
+    </row>
+    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D193" s="2"/>
+      <c r="E193" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F193" s="2"/>
+      <c r="G193" s="2"/>
+      <c r="H193" s="2"/>
+      <c r="I193" s="2"/>
+      <c r="J193" s="2"/>
+      <c r="K193" s="2"/>
+      <c r="L193" s="2"/>
+      <c r="N193" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O193" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P193" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q193" s="8"/>
+      <c r="R193" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="S193" s="8"/>
+      <c r="T193" s="8"/>
+      <c r="U193" s="8"/>
+      <c r="V193" s="8"/>
+      <c r="W193" s="8"/>
+      <c r="X193" s="8"/>
+      <c r="Y193" s="8"/>
+    </row>
+    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A194" s="2"/>
+      <c r="B194" s="2"/>
+      <c r="C194" s="2"/>
+      <c r="D194" s="2"/>
+      <c r="E194" s="2"/>
+      <c r="F194" s="2"/>
+      <c r="G194" s="2"/>
+      <c r="H194" s="2"/>
+      <c r="I194" s="2"/>
+      <c r="J194" s="2"/>
+      <c r="K194" s="2"/>
+      <c r="L194" s="2"/>
+      <c r="N194" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O194" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P194" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q194" s="8"/>
+      <c r="R194" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S194" s="8"/>
+      <c r="T194" s="8"/>
+      <c r="U194" s="8"/>
+      <c r="V194" s="8"/>
+      <c r="W194" s="8"/>
+      <c r="X194" s="8"/>
+      <c r="Y194" s="8"/>
+    </row>
+    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+      <c r="D198" s="1"/>
+      <c r="E198" s="1"/>
+      <c r="F198" s="1"/>
+      <c r="G198" s="1"/>
+      <c r="H198" s="1"/>
+    </row>
+    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1"/>
+      <c r="E199" s="1"/>
+      <c r="F199" s="1"/>
+      <c r="G199" s="1"/>
+      <c r="H199" s="1"/>
+    </row>
+    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
+      <c r="C200" s="1"/>
+      <c r="D200" s="1"/>
+      <c r="E200" s="1"/>
+      <c r="F200" s="1"/>
+      <c r="G200" s="1"/>
+      <c r="H200" s="1"/>
+    </row>
+    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+      <c r="D201" s="1"/>
+      <c r="E201" s="1"/>
+      <c r="F201" s="1"/>
+      <c r="G201" s="1"/>
+      <c r="H201" s="1"/>
+    </row>
+    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A202" s="1"/>
+      <c r="B202" s="1"/>
+      <c r="C202" s="1"/>
+      <c r="D202" s="1"/>
+      <c r="E202" s="1"/>
+      <c r="F202" s="1"/>
+      <c r="G202" s="1"/>
+      <c r="H202" s="1"/>
+    </row>
+    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+      <c r="D203" s="1"/>
+      <c r="E203" s="1"/>
+      <c r="F203" s="1"/>
+      <c r="G203" s="1"/>
+      <c r="H203" s="1"/>
+    </row>
+    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="1"/>
+      <c r="F204" s="1"/>
+      <c r="G204" s="1"/>
+      <c r="H204" s="1"/>
+    </row>
+    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="1"/>
+      <c r="D205" s="1"/>
+      <c r="E205" s="1"/>
+      <c r="F205" s="1"/>
+      <c r="G205" s="1"/>
+      <c r="H205" s="1"/>
+    </row>
+    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A206" s="1"/>
+      <c r="B206" s="1"/>
+      <c r="C206" s="1"/>
+      <c r="D206" s="1"/>
+      <c r="E206" s="1"/>
+      <c r="F206" s="1"/>
+      <c r="G206" s="1"/>
+      <c r="H206" s="1"/>
+    </row>
+    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G207" s="1"/>
+      <c r="H207" s="1"/>
+    </row>
+    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D208" s="1"/>
+      <c r="E208" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F208" s="1"/>
+      <c r="G208" s="1"/>
+      <c r="H208" s="1"/>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="1"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D210" s="1"/>
+      <c r="E210" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F210" s="1"/>
+      <c r="G210" s="1"/>
+      <c r="H210" s="1"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F211" s="1"/>
+      <c r="G211" s="1"/>
+      <c r="H211" s="1"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D212" s="1"/>
+      <c r="E212" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F212" s="1"/>
+      <c r="G212" s="1"/>
+      <c r="H212" s="1"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A213" s="1"/>
+      <c r="B213" s="1"/>
+      <c r="C213" s="1"/>
+      <c r="D213" s="1"/>
+      <c r="E213" s="1"/>
+      <c r="F213" s="1"/>
+      <c r="G213" s="1"/>
+      <c r="H213" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>